<commit_message>
Updated to version 2016-04-29
</commit_message>
<xml_diff>
--- a/SolvencyII.UI/SolvencyII.ExcelImportExportLib/ExcelTemplates/BusinessTemplates/afb_annual_financial_stability_third_country_branches.xlsx
+++ b/SolvencyII.UI/SolvencyII.ExcelImportExportLib/ExcelTemplates/BusinessTemplates/afb_annual_financial_stability_third_country_branches.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremi Kiraga\Desktop\business\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jeremi Kiraga\Desktop\ExcelGenCmd\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="7245"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="8550"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="3" r:id="rId1"/>
@@ -52,7 +52,7 @@
     <definedName name="S.40.01.10.01.TD" localSheetId="8">S.40.01.10.01!$C$6:$D$7</definedName>
     <definedName name="Version" localSheetId="0">Info!$B$2:$C$4</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -130,7 +130,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>Ver:2016.02.29</t>
+    <t>Ver:2016.04.18</t>
   </si>
   <si>
     <t>Back to TOC</t>
@@ -931,13 +931,13 @@
     <t>Name of a branch</t>
   </si>
   <si>
-    <t>C0030</t>
+    <t>R0000C0030</t>
   </si>
   <si>
     <t>Country of a branch</t>
   </si>
   <si>
-    <t>C0040</t>
+    <t>R0000C0040</t>
   </si>
   <si>
     <t>C0020</t>
@@ -2283,7 +2283,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd\-mm\-yyyy"/>
+    <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -2291,6 +2291,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2299,6 +2300,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2307,6 +2309,7 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2314,6 +2317,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -2723,9 +2727,9 @@
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -2775,9 +2779,9 @@
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -2980,9 +2984,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="50.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6241,9 +6245,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
+    <col min="4" max="4" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -6368,9 +6372,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -6486,9 +6490,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -6780,9 +6784,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -6855,10 +6859,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="35" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="33" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="35" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="24" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -6950,10 +6954,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" style="31" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" style="25" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" style="29" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="31" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="25" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" style="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -7043,9 +7047,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -7117,9 +7121,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.5703125" customWidth="1"/>
-    <col min="2" max="2" width="50.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="50.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:9" x14ac:dyDescent="0.25">
@@ -7177,6 +7181,6 @@
     <hyperlink ref="B1" location="'Table of contents'!A1" tooltip="Click to navigate Table of contents" display="Back to TOC"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>